<commit_message>
Added more admin commands
</commit_message>
<xml_diff>
--- a/MakerRanger/Docs/MakerRangerTags.xlsx
+++ b/MakerRanger/Docs/MakerRangerTags.xlsx
@@ -24,19 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
-  <si>
-    <t>hippopotamus</t>
-  </si>
-  <si>
-    <t>penguin</t>
-  </si>
-  <si>
-    <t>monkey</t>
-  </si>
-  <si>
-    <t>sheep</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>Rabbit</t>
   </si>
@@ -146,9 +134,6 @@
     <t>94785B2E</t>
   </si>
   <si>
-    <t xml:space="preserve">84AA732E </t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -216,6 +201,54 @@
   </si>
   <si>
     <t>B7538CF4</t>
+  </si>
+  <si>
+    <t>67668FF4</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Reprint</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>AbortGame</t>
+  </si>
+  <si>
+    <t>677C36F4</t>
+  </si>
+  <si>
+    <t>Rounds</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Hippopotamus</t>
+  </si>
+  <si>
+    <t>Penguin</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>77B322F4</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>84AA732E</t>
   </si>
 </sst>
 </file>
@@ -534,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,13 +584,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" t="str">
         <f>CONCATENATE(C1,CHAR(9),B1,"|",A1)</f>
@@ -568,94 +601,94 @@
         <v>Hare</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D33" si="0">CONCATENATE(C2,CHAR(9),B2,"|",A2)</f>
-        <v>F7C68DF4	01|monkey</v>
+        <v>F7C68DF4	01|Monkey</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E33" si="1">LEFT(A2,16)</f>
-        <v>monkey</v>
+        <v>Monkey</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>D7965CF4	02|penguin</v>
+        <v>D7965CF4	02|Penguin</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
-        <v>penguin</v>
+        <v>Penguin</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>A49E502E	03|hippopotamus</v>
+        <v>A49E502E	03|Hippopotamus</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>hippopotamus</v>
+        <v>Hippopotamus</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>87DC8CF4	04|sheep</v>
+        <v>87DC8CF4	04|Sheep</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>sheep</v>
+        <v>Sheep</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -668,13 +701,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -687,13 +720,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -706,35 +739,35 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>4460792E	08|Bee</v>
+        <v>87AA36F4	08|Bee</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
         <v>Bee</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -745,18 +778,18 @@
         <v>Elephant</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -769,13 +802,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -788,13 +821,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -807,13 +840,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -826,13 +859,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -857,13 +890,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -876,89 +909,89 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>775228F4	01|monkey</v>
+        <v>775228F4	01|Monkey</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>monkey</v>
+        <v>Monkey</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>671931F4	02|penguin</v>
+        <v>671931F4	02|Penguin</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>penguin</v>
+        <v>Penguin</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>97602CF4	03|hippopotamus</v>
+        <v>97602CF4	03|Hippopotamus</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>hippopotamus</v>
+        <v>Hippopotamus</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>A7748EF4	04|sheep</v>
+        <v>A7748EF4	04|Sheep</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>sheep</v>
+        <v>Sheep</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -971,13 +1004,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -990,13 +1023,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -1009,13 +1042,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -1028,13 +1061,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -1047,13 +1080,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -1066,13 +1099,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -1085,13 +1118,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -1104,13 +1137,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -1123,13 +1156,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -1154,21 +1187,97 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>84AA732E 	100|Player</v>
+        <v>84AA732E	100|Reprint</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
+        <v>Reprint</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34" si="2">CONCATENATE(C34,CHAR(9),B34,"|",A34)</f>
+        <v>67668FF4	101|AbortGame</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" ref="E34:E35" si="3">LEFT(A34,16)</f>
+        <v>AbortGame</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35" si="4">CONCATENATE(C35,CHAR(9),B35,"|",A35)</f>
+        <v>677C36F4	102|Player</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" ref="E35:E36" si="5">LEFT(A35,16)</f>
         <v>Player</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ref="D36" si="6">CONCATENATE(C36,CHAR(9),B36,"|",A36)</f>
+        <v>4460792E	103|Rounds</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" ref="E36" si="7">LEFT(A36,16)</f>
+        <v>Rounds</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D37" si="8">CONCATENATE(C37,CHAR(9),B37,"|",A37)</f>
+        <v>77B322F4	104|Show</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" ref="E37" si="9">LEFT(A37,16)</f>
+        <v>Show</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web server integration added
</commit_message>
<xml_diff>
--- a/MakerRanger/Docs/MakerRangerTags.xlsx
+++ b/MakerRanger/Docs/MakerRangerTags.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
   <si>
     <t>Rabbit</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>84AA732E</t>
+  </si>
+  <si>
+    <t>D7BE2FF4</t>
+  </si>
+  <si>
+    <t>A7C683F4</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,11 +621,11 @@
         <v>12</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D33" si="0">CONCATENATE(C2,CHAR(9),B2,"|",A2)</f>
+        <f t="shared" ref="D2:D35" si="0">CONCATENATE(C2,CHAR(9),B2,"|",A2)</f>
         <v>F7C68DF4	01|Monkey</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="1">LEFT(A2,16)</f>
+        <f t="shared" ref="E2:E35" si="1">LEFT(A2,16)</f>
         <v>Monkey</v>
       </c>
     </row>
@@ -1174,109 +1180,147 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">	|</v>
+        <f t="shared" ref="D32:D33" si="2">CONCATENATE(C32,CHAR(9),B32,"|",A32)</f>
+        <v>A7C683F4	10|GingerBreadMan</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" ref="E32:E33" si="3">LEFT(A32,16)</f>
+        <v>GingerBreadMan</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>84AA732E	100|Reprint</v>
+        <f t="shared" si="2"/>
+        <v>D7BE2FF4	10|GingerBreadMan</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>Reprint</v>
+        <f t="shared" si="3"/>
+        <v>GingerBreadMan</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" t="str">
-        <f t="shared" ref="D34" si="2">CONCATENATE(C34,CHAR(9),B34,"|",A34)</f>
-        <v>67668FF4	101|AbortGame</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">	|</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E35" si="3">LEFT(A34,16)</f>
-        <v>AbortGame</v>
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" ref="D35" si="4">CONCATENATE(C35,CHAR(9),B35,"|",A35)</f>
-        <v>677C36F4	102|Player</v>
+        <f t="shared" si="0"/>
+        <v>84AA732E	100|Reprint</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" ref="E35:E36" si="5">LEFT(A35,16)</f>
-        <v>Player</v>
+        <f t="shared" si="1"/>
+        <v>Reprint</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" ref="D36" si="6">CONCATENATE(C36,CHAR(9),B36,"|",A36)</f>
-        <v>4460792E	103|Rounds</v>
+        <f t="shared" ref="D36" si="4">CONCATENATE(C36,CHAR(9),B36,"|",A36)</f>
+        <v>67668FF4	101|AbortGame</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" ref="E36" si="7">LEFT(A36,16)</f>
-        <v>Rounds</v>
+        <f t="shared" ref="E36" si="5">LEFT(A36,16)</f>
+        <v>AbortGame</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D37" si="6">CONCATENATE(C37,CHAR(9),B37,"|",A37)</f>
+        <v>677C36F4	102|Player</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" ref="E37" si="7">LEFT(A37,16)</f>
+        <v>Player</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" ref="D38" si="8">CONCATENATE(C38,CHAR(9),B38,"|",A38)</f>
+        <v>4460792E	103|Rounds</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" ref="E38" si="9">LEFT(A38,16)</f>
+        <v>Rounds</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D37" t="str">
-        <f t="shared" ref="D37" si="8">CONCATENATE(C37,CHAR(9),B37,"|",A37)</f>
+      <c r="D39" t="str">
+        <f t="shared" ref="D39" si="10">CONCATENATE(C39,CHAR(9),B39,"|",A39)</f>
         <v>77B322F4	104|Show</v>
       </c>
-      <c r="E37" t="str">
-        <f t="shared" ref="E37" si="9">LEFT(A37,16)</f>
+      <c r="E39" t="str">
+        <f t="shared" ref="E39" si="11">LEFT(A39,16)</f>
         <v>Show</v>
       </c>
     </row>

</xml_diff>